<commit_message>
add metadata to spreadsheet
</commit_message>
<xml_diff>
--- a/src/test_data/simple_dental_data_specification.xlsx
+++ b/src/test_data/simple_dental_data_specification.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="57800" yWindow="720" windowWidth="42940" windowHeight="19520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="47">
   <si>
     <t>data_source</t>
   </si>
@@ -148,6 +148,18 @@
   </si>
   <si>
     <t>amalgam restoration</t>
+  </si>
+  <si>
+    <t>tooth 1</t>
+  </si>
+  <si>
+    <t>tooth 2</t>
+  </si>
+  <si>
+    <t>tooth 3</t>
+  </si>
+  <si>
+    <t>tooth 4</t>
   </si>
 </sst>
 </file>
@@ -536,7 +548,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -632,6 +644,9 @@
       <c r="D5" t="s">
         <v>27</v>
       </c>
+      <c r="E5" t="s">
+        <v>43</v>
+      </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
@@ -649,6 +664,9 @@
       <c r="D6" t="s">
         <v>28</v>
       </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
       <c r="F6" t="s">
         <v>8</v>
       </c>
@@ -666,6 +684,9 @@
       <c r="D7" t="s">
         <v>29</v>
       </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
       <c r="F7" t="s">
         <v>8</v>
       </c>
@@ -682,6 +703,9 @@
       </c>
       <c r="D8" t="s">
         <v>30</v>
+      </c>
+      <c r="E8" t="s">
+        <v>46</v>
       </c>
       <c r="F8" t="s">
         <v>8</v>

</xml_diff>